<commit_message>
AREA MA, AREA PPQA
Se actualizaron las metricas y se ordenaron en sus respectivas areas.
</commit_message>
<xml_diff>
--- a/Area PPQA/F.DEV90.PPQA.R03 -Registro de resultados de métricas.xlsx
+++ b/Area PPQA/F.DEV90.PPQA.R03 -Registro de resultados de métricas.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="21195" windowHeight="9975"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20640" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nombre de Metrica</t>
   </si>
@@ -49,13 +49,28 @@
   </si>
   <si>
     <t>Numero de no Conformidades QA del Producto</t>
+  </si>
+  <si>
+    <t>Porcentajes de Cumplimiento de Entregable</t>
+  </si>
+  <si>
+    <t>Volatibilidad de Requerimientos</t>
+  </si>
+  <si>
+    <t>PP_PMC</t>
+  </si>
+  <si>
+    <t>REQM</t>
+  </si>
+  <si>
+    <t>Mes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,8 +84,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,8 +106,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -92,14 +127,268 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B11:I13"/>
+  <dimension ref="B2:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B11:B12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,56 +702,117 @@
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I4" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="K4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-      <c r="E13">
-        <v>15</v>
-      </c>
-      <c r="H13">
-        <v>12.5</v>
-      </c>
-      <c r="I13" s="1"/>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <f>(D5+E5+F5+G5)/2</f>
+        <v>2</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7">
+        <v>6</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="18">
+        <f>(D6+E6+F6+G6)/12</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="18">
+        <f>(D7+E7+F7+G7)/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="I7" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:I3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>